<commit_message>
background colors for plots in place
</commit_message>
<xml_diff>
--- a/Notes/Color-palette.xlsx
+++ b/Notes/Color-palette.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Homework\Interactive-Visualization-and-Dashboard-Challenge\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Homework\Interactive-Visualization-and-Dashboard-Challenge\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="290">
   <si>
     <t>RGB hex value</t>
   </si>
@@ -911,6 +911,9 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
@@ -2234,9 +2237,6 @@
     <xf numFmtId="0" fontId="2" fillId="139" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2245,6 +2245,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2563,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2602,7 +2605,7 @@
       <c r="J2" s="62"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B3" s="145"/>
+      <c r="B3" s="148"/>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2615,7 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B4" s="145"/>
+      <c r="B4" s="148"/>
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
@@ -2629,7 +2632,7 @@
       <c r="J4" s="97"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B5" s="145"/>
+      <c r="B5" s="148"/>
       <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
@@ -2646,7 +2649,7 @@
       <c r="J5" s="123"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B6" s="145"/>
+      <c r="B6" s="148"/>
       <c r="C6" s="4" t="s">
         <v>189</v>
       </c>
@@ -2663,7 +2666,7 @@
       <c r="J6" s="46"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B7" s="145"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
@@ -2680,7 +2683,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B8" s="145"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="4" t="s">
         <v>79</v>
       </c>
@@ -2697,7 +2700,7 @@
       <c r="J8" s="103"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B9" s="145"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2714,7 +2717,7 @@
       <c r="J9" s="72"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B10" s="145"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
@@ -2731,7 +2734,7 @@
       <c r="O10" s="125"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B11" s="145"/>
+      <c r="B11" s="148"/>
       <c r="C11" s="4" t="s">
         <v>73</v>
       </c>
@@ -2748,7 +2751,7 @@
       <c r="O11" s="43"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B12" s="145"/>
+      <c r="B12" s="148"/>
       <c r="C12" s="4" t="s">
         <v>109</v>
       </c>
@@ -2765,7 +2768,7 @@
       <c r="O12" s="119"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B13" s="145"/>
+      <c r="B13" s="148"/>
       <c r="C13" s="4" t="s">
         <v>103</v>
       </c>
@@ -2789,7 +2792,7 @@
       <c r="O13" s="35"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B14" s="145"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="4" t="s">
         <v>199</v>
       </c>
@@ -2813,7 +2816,7 @@
       <c r="O14" s="111"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B15" s="145"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
@@ -2837,7 +2840,7 @@
       <c r="O15" s="139"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B16" s="145"/>
+      <c r="B16" s="148"/>
       <c r="C16" s="4" t="s">
         <v>268</v>
       </c>
@@ -2861,7 +2864,7 @@
       <c r="O16" s="36"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B17" s="145"/>
+      <c r="B17" s="148"/>
       <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
@@ -2878,14 +2881,14 @@
       <c r="O17" s="49"/>
     </row>
     <row r="18" spans="2:21" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="145"/>
+      <c r="B18" s="148"/>
       <c r="C18" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="146" t="s">
+      <c r="D18" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="147"/>
+      <c r="E18" s="146"/>
       <c r="H18" s="4" t="s">
         <v>229</v>
       </c>
@@ -2933,7 +2936,7 @@
       <c r="O19" s="87"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B20" s="145"/>
+      <c r="B20" s="148"/>
       <c r="C20" s="4" t="s">
         <v>114</v>
       </c>
@@ -2950,7 +2953,7 @@
       <c r="J20" s="65"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B21" s="145"/>
+      <c r="B21" s="148"/>
       <c r="C21" s="4" t="s">
         <v>170</v>
       </c>
@@ -2967,7 +2970,7 @@
       <c r="J21" s="121"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B22" s="145"/>
+      <c r="B22" s="148"/>
       <c r="C22" s="4" t="s">
         <v>120</v>
       </c>
@@ -2984,7 +2987,7 @@
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B23" s="145"/>
+      <c r="B23" s="148"/>
       <c r="C23" s="4" t="s">
         <v>253</v>
       </c>
@@ -3008,7 +3011,7 @@
       <c r="O23" s="137"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B24" s="145"/>
+      <c r="B24" s="148"/>
       <c r="C24" s="4" t="s">
         <v>100</v>
       </c>
@@ -3025,7 +3028,7 @@
       <c r="J24" s="76"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B25" s="145"/>
+      <c r="B25" s="148"/>
       <c r="C25" s="4" t="s">
         <v>102</v>
       </c>
@@ -3042,7 +3045,7 @@
       <c r="J25" s="52"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B26" s="145"/>
+      <c r="B26" s="148"/>
       <c r="C26" s="4" t="s">
         <v>181</v>
       </c>
@@ -3059,7 +3062,7 @@
       <c r="J26" s="141"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B27" s="145"/>
+      <c r="B27" s="148"/>
       <c r="C27" s="4" t="s">
         <v>195</v>
       </c>
@@ -3076,7 +3079,7 @@
       <c r="J27" s="113"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B28" s="145"/>
+      <c r="B28" s="148"/>
       <c r="C28" s="4" t="s">
         <v>278</v>
       </c>
@@ -3093,7 +3096,7 @@
       <c r="J28" s="81"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B29" s="145"/>
+      <c r="B29" s="148"/>
       <c r="C29" s="4" t="s">
         <v>245</v>
       </c>
@@ -3110,7 +3113,7 @@
       <c r="J29" s="75"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B30" s="145"/>
+      <c r="B30" s="148"/>
       <c r="C30" s="4" t="s">
         <v>270</v>
       </c>
@@ -3127,7 +3130,7 @@
       <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B31" s="145"/>
+      <c r="B31" s="148"/>
       <c r="C31" s="4" t="s">
         <v>98</v>
       </c>
@@ -3144,7 +3147,7 @@
       <c r="J31" s="70"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.45">
-      <c r="B32" s="145"/>
+      <c r="B32" s="148"/>
       <c r="C32" s="4" t="s">
         <v>201</v>
       </c>
@@ -3160,8 +3163,8 @@
       </c>
       <c r="J32" s="26"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B33" s="145"/>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B33" s="148"/>
       <c r="C33" s="4" t="s">
         <v>139</v>
       </c>
@@ -3177,8 +3180,8 @@
       </c>
       <c r="J33" s="127"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B34" s="145"/>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B34" s="148"/>
       <c r="C34" s="4" t="s">
         <v>86</v>
       </c>
@@ -3194,8 +3197,8 @@
       </c>
       <c r="J34" s="142"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B35" s="145"/>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B35" s="148"/>
       <c r="C35" s="4" t="s">
         <v>56</v>
       </c>
@@ -3211,8 +3214,8 @@
       </c>
       <c r="J35" s="27"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B36" s="145"/>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B36" s="148"/>
       <c r="C36" s="4" t="s">
         <v>64</v>
       </c>
@@ -3228,8 +3231,8 @@
       </c>
       <c r="J36" s="143"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B37" s="145"/>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B37" s="148"/>
       <c r="C37" s="4" t="s">
         <v>187</v>
       </c>
@@ -3245,8 +3248,8 @@
       </c>
       <c r="J37" s="105"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B38" s="145"/>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B38" s="148"/>
       <c r="C38" s="4" t="s">
         <v>111</v>
       </c>
@@ -3262,8 +3265,8 @@
       </c>
       <c r="J38" s="66"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B39" s="145"/>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B39" s="148"/>
       <c r="C39" s="4" t="s">
         <v>113</v>
       </c>
@@ -3279,8 +3282,8 @@
       </c>
       <c r="J39" s="126"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B40" s="145"/>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B40" s="148"/>
       <c r="C40" s="4" t="s">
         <v>261</v>
       </c>
@@ -3295,9 +3298,12 @@
         <v>39</v>
       </c>
       <c r="J40" s="24"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B41" s="145"/>
+      <c r="L40" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B41" s="148"/>
       <c r="C41" s="4" t="s">
         <v>217</v>
       </c>
@@ -3313,8 +3319,8 @@
       </c>
       <c r="J41" s="94"/>
     </row>
-    <row r="42" spans="2:10" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B42" s="145"/>
+    <row r="42" spans="2:12" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="B42" s="148"/>
       <c r="C42" s="4" t="s">
         <v>263</v>
       </c>
@@ -3330,8 +3336,8 @@
       </c>
       <c r="J42" s="83"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B43" s="145"/>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B43" s="148"/>
       <c r="C43" s="4" t="s">
         <v>265</v>
       </c>
@@ -3347,8 +3353,8 @@
       </c>
       <c r="J43" s="109"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B44" s="145"/>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B44" s="148"/>
       <c r="C44" s="4" t="s">
         <v>174</v>
       </c>
@@ -3364,8 +3370,8 @@
       </c>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B45" s="145"/>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B45" s="148"/>
       <c r="C45" s="4" t="s">
         <v>176</v>
       </c>
@@ -3381,8 +3387,8 @@
       </c>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B46" s="145"/>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B46" s="148"/>
       <c r="C46" s="4" t="s">
         <v>197</v>
       </c>
@@ -3393,13 +3399,13 @@
       <c r="H46" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I46" s="146" t="s">
+      <c r="I46" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="148"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B47" s="145"/>
+      <c r="J46" s="147"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B47" s="148"/>
       <c r="C47" s="4" t="s">
         <v>149</v>
       </c>
@@ -3415,8 +3421,8 @@
       </c>
       <c r="J47" s="58"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B48" s="145"/>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B48" s="148"/>
       <c r="C48" s="4" t="s">
         <v>58</v>
       </c>
@@ -3426,7 +3432,7 @@
       <c r="E48" s="34"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B49" s="145"/>
+      <c r="B49" s="148"/>
       <c r="C49" s="4" t="s">
         <v>40</v>
       </c>
@@ -3436,7 +3442,7 @@
       <c r="E49" s="25"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B50" s="145"/>
+      <c r="B50" s="148"/>
       <c r="C50" s="4" t="s">
         <v>10</v>
       </c>
@@ -3446,7 +3452,7 @@
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B51" s="145"/>
+      <c r="B51" s="148"/>
       <c r="C51" s="4" t="s">
         <v>14</v>
       </c>
@@ -3456,7 +3462,7 @@
       <c r="E51" s="12"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B52" s="145"/>
+      <c r="B52" s="148"/>
       <c r="C52" s="4" t="s">
         <v>22</v>
       </c>
@@ -3466,7 +3472,7 @@
       <c r="E52" s="16"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B53" s="145"/>
+      <c r="B53" s="148"/>
       <c r="C53" s="4" t="s">
         <v>6</v>
       </c>
@@ -3476,7 +3482,7 @@
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B54" s="145"/>
+      <c r="B54" s="148"/>
       <c r="C54" s="4" t="s">
         <v>132</v>
       </c>
@@ -3486,7 +3492,7 @@
       <c r="E54" s="9"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B55" s="145"/>
+      <c r="B55" s="148"/>
       <c r="C55" s="4" t="s">
         <v>259</v>
       </c>
@@ -3496,7 +3502,7 @@
       <c r="E55" s="131"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B56" s="145"/>
+      <c r="B56" s="148"/>
       <c r="C56" s="4" t="s">
         <v>172</v>
       </c>
@@ -3506,7 +3512,7 @@
       <c r="E56" s="89"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B57" s="145"/>
+      <c r="B57" s="148"/>
       <c r="C57" s="4" t="s">
         <v>50</v>
       </c>
@@ -3516,7 +3522,7 @@
       <c r="E57" s="30"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B58" s="145"/>
+      <c r="B58" s="148"/>
       <c r="C58" s="4" t="s">
         <v>92</v>
       </c>
@@ -3533,7 +3539,7 @@
       <c r="J58" s="71"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B59" s="145"/>
+      <c r="B59" s="148"/>
       <c r="C59" s="4" t="s">
         <v>84</v>
       </c>
@@ -3543,10 +3549,10 @@
       <c r="E59" s="47"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B60" s="145"/>
+      <c r="B60" s="148"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B61" s="145"/>
+      <c r="B61" s="148"/>
       <c r="C61" s="4" t="s">
         <v>96</v>
       </c>
@@ -3556,7 +3562,7 @@
       <c r="E61" s="53"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B62" s="145"/>
+      <c r="B62" s="148"/>
       <c r="C62" s="4" t="s">
         <v>163</v>
       </c>
@@ -3566,7 +3572,7 @@
       <c r="E62" s="84"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B63" s="145"/>
+      <c r="B63" s="148"/>
       <c r="C63" s="4" t="s">
         <v>193</v>
       </c>
@@ -3576,7 +3582,7 @@
       <c r="E63" s="98"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B64" s="145"/>
+      <c r="B64" s="148"/>
       <c r="C64" s="4" t="s">
         <v>105</v>
       </c>
@@ -3586,7 +3592,7 @@
       <c r="E64" s="57"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B65" s="145"/>
+      <c r="B65" s="148"/>
       <c r="C65" s="4" t="s">
         <v>225</v>
       </c>
@@ -3596,7 +3602,7 @@
       <c r="E65" s="114"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B66" s="145"/>
+      <c r="B66" s="148"/>
       <c r="C66" s="4" t="s">
         <v>90</v>
       </c>
@@ -3606,7 +3612,7 @@
       <c r="E66" s="50"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B67" s="145"/>
+      <c r="B67" s="148"/>
       <c r="C67" s="4" t="s">
         <v>286</v>
       </c>
@@ -3616,7 +3622,7 @@
       <c r="E67" s="144"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B68" s="145"/>
+      <c r="B68" s="148"/>
       <c r="C68" s="4" t="s">
         <v>257</v>
       </c>
@@ -3626,7 +3632,7 @@
       <c r="E68" s="130"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B69" s="145"/>
+      <c r="B69" s="148"/>
       <c r="C69" s="4" t="s">
         <v>52</v>
       </c>
@@ -3636,7 +3642,7 @@
       <c r="E69" s="31"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B70" s="145"/>
+      <c r="B70" s="148"/>
       <c r="C70" s="4" t="s">
         <v>77</v>
       </c>
@@ -3646,7 +3652,7 @@
       <c r="E70" s="44"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B71" s="145"/>
+      <c r="B71" s="148"/>
       <c r="C71" s="4" t="s">
         <v>81</v>
       </c>
@@ -3656,7 +3662,7 @@
       <c r="E71" s="9"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B72" s="145"/>
+      <c r="B72" s="148"/>
       <c r="C72" s="4" t="s">
         <v>153</v>
       </c>
@@ -3666,7 +3672,7 @@
       <c r="E72" s="80"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B73" s="145"/>
+      <c r="B73" s="148"/>
       <c r="C73" s="4" t="s">
         <v>130</v>
       </c>
@@ -3676,7 +3682,7 @@
       <c r="E73" s="69"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B74" s="145"/>
+      <c r="B74" s="148"/>
       <c r="C74" s="4" t="s">
         <v>227</v>
       </c>
@@ -3686,7 +3692,7 @@
       <c r="E74" s="115"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B75" s="145"/>
+      <c r="B75" s="148"/>
       <c r="C75" s="4" t="s">
         <v>177</v>
       </c>
@@ -3696,7 +3702,7 @@
       <c r="E75" s="91"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B76" s="145"/>
+      <c r="B76" s="148"/>
       <c r="C76" s="4" t="s">
         <v>241</v>
       </c>
@@ -3706,7 +3712,7 @@
       <c r="E76" s="122"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B77" s="145"/>
+      <c r="B77" s="148"/>
       <c r="C77" s="4" t="s">
         <v>116</v>
       </c>
@@ -3716,7 +3722,7 @@
       <c r="E77" s="62"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B78" s="145"/>
+      <c r="B78" s="148"/>
       <c r="C78" s="4" t="s">
         <v>75</v>
       </c>
@@ -3726,7 +3732,7 @@
       <c r="E78" s="43"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B79" s="145"/>
+      <c r="B79" s="148"/>
       <c r="C79" s="4" t="s">
         <v>191</v>
       </c>
@@ -3736,7 +3742,7 @@
       <c r="E79" s="97"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B80" s="145"/>
+      <c r="B80" s="148"/>
       <c r="C80" s="4" t="s">
         <v>243</v>
       </c>
@@ -3746,7 +3752,7 @@
       <c r="E80" s="123"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B81" s="145"/>
+      <c r="B81" s="148"/>
       <c r="C81" s="4" t="s">
         <v>82</v>
       </c>
@@ -3756,7 +3762,7 @@
       <c r="E81" s="46"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B82" s="145"/>
+      <c r="B82" s="148"/>
       <c r="C82" s="4" t="s">
         <v>4</v>
       </c>
@@ -3766,7 +3772,7 @@
       <c r="E82" s="7"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B83" s="145"/>
+      <c r="B83" s="148"/>
       <c r="C83" s="4" t="s">
         <v>203</v>
       </c>
@@ -3776,7 +3782,7 @@
       <c r="E83" s="103"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B84" s="145"/>
+      <c r="B84" s="148"/>
       <c r="C84" s="4" t="s">
         <v>137</v>
       </c>
@@ -3786,7 +3792,7 @@
       <c r="E84" s="72"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B85" s="145"/>
+      <c r="B85" s="148"/>
       <c r="C85" s="4" t="s">
         <v>235</v>
       </c>
@@ -3796,7 +3802,7 @@
       <c r="E85" s="119"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B86" s="145"/>
+      <c r="B86" s="148"/>
       <c r="C86" s="4" t="s">
         <v>60</v>
       </c>
@@ -3806,7 +3812,7 @@
       <c r="E86" s="35"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B87" s="145"/>
+      <c r="B87" s="148"/>
       <c r="C87" s="4" t="s">
         <v>272</v>
       </c>
@@ -3816,7 +3822,7 @@
       <c r="E87" s="137"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B88" s="145"/>
+      <c r="B88" s="148"/>
       <c r="C88" s="4" t="s">
         <v>161</v>
       </c>
@@ -3826,7 +3832,7 @@
       <c r="E88" s="9"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B89" s="145"/>
+      <c r="B89" s="148"/>
       <c r="C89" s="4" t="s">
         <v>165</v>
       </c>
@@ -3836,7 +3842,7 @@
       <c r="E89" s="85"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B90" s="145"/>
+      <c r="B90" s="148"/>
       <c r="C90" s="4" t="s">
         <v>274</v>
       </c>
@@ -3846,7 +3852,7 @@
       <c r="E90" s="138"/>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B91" s="145"/>
+      <c r="B91" s="148"/>
       <c r="C91" s="4" t="s">
         <v>221</v>
       </c>
@@ -3856,7 +3862,7 @@
       <c r="E91" s="112"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B92" s="145"/>
+      <c r="B92" s="148"/>
       <c r="C92" s="4" t="s">
         <v>128</v>
       </c>
@@ -3866,7 +3872,7 @@
       <c r="E92" s="68"/>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B93" s="145"/>
+      <c r="B93" s="148"/>
       <c r="C93" s="4" t="s">
         <v>229</v>
       </c>
@@ -3876,7 +3882,7 @@
       <c r="E93" s="116"/>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B94" s="145"/>
+      <c r="B94" s="148"/>
       <c r="C94" s="4" t="s">
         <v>68</v>
       </c>
@@ -3886,7 +3892,7 @@
       <c r="E94" s="39"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B95" s="145"/>
+      <c r="B95" s="148"/>
       <c r="C95" s="4" t="s">
         <v>122</v>
       </c>
@@ -3896,7 +3902,7 @@
       <c r="E95" s="65"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B96" s="145"/>
+      <c r="B96" s="148"/>
       <c r="C96" s="4" t="s">
         <v>239</v>
       </c>
@@ -3906,7 +3912,7 @@
       <c r="E96" s="121"/>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B97" s="145"/>
+      <c r="B97" s="148"/>
       <c r="C97" s="4" t="s">
         <v>54</v>
       </c>
@@ -3916,7 +3922,7 @@
       <c r="E97" s="32"/>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B98" s="145"/>
+      <c r="B98" s="148"/>
       <c r="C98" s="4" t="s">
         <v>157</v>
       </c>
@@ -3926,7 +3932,7 @@
       <c r="E98" s="82"/>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B99" s="145"/>
+      <c r="B99" s="148"/>
       <c r="C99" s="4" t="s">
         <v>145</v>
       </c>
@@ -3936,7 +3942,7 @@
       <c r="E99" s="76"/>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B100" s="145"/>
+      <c r="B100" s="148"/>
       <c r="C100" s="4" t="s">
         <v>94</v>
       </c>
@@ -3946,7 +3952,7 @@
       <c r="E100" s="52"/>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B101" s="145"/>
+      <c r="B101" s="148"/>
       <c r="C101" s="4" t="s">
         <v>280</v>
       </c>
@@ -3956,7 +3962,7 @@
       <c r="E101" s="141"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B102" s="145"/>
+      <c r="B102" s="148"/>
       <c r="C102" s="4" t="s">
         <v>223</v>
       </c>
@@ -3966,7 +3972,7 @@
       <c r="E102" s="113"/>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B103" s="145"/>
+      <c r="B103" s="148"/>
       <c r="C103" s="4" t="s">
         <v>155</v>
       </c>
@@ -3976,7 +3982,7 @@
       <c r="E103" s="81"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B104" s="145"/>
+      <c r="B104" s="148"/>
       <c r="C104" s="4" t="s">
         <v>143</v>
       </c>
@@ -3986,7 +3992,7 @@
       <c r="E104" s="75"/>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B105" s="145"/>
+      <c r="B105" s="148"/>
       <c r="C105" s="4" t="s">
         <v>36</v>
       </c>
@@ -3996,7 +4002,7 @@
       <c r="E105" s="23"/>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B106" s="145"/>
+      <c r="B106" s="148"/>
       <c r="C106" s="4" t="s">
         <v>133</v>
       </c>
@@ -4006,7 +4012,7 @@
       <c r="E106" s="70"/>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B107" s="145"/>
+      <c r="B107" s="148"/>
       <c r="C107" s="4" t="s">
         <v>42</v>
       </c>
@@ -4016,7 +4022,7 @@
       <c r="E107" s="26"/>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B108" s="145"/>
+      <c r="B108" s="148"/>
       <c r="C108" s="4" t="s">
         <v>251</v>
       </c>
@@ -4026,7 +4032,7 @@
       <c r="E108" s="127"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B109" s="145"/>
+      <c r="B109" s="148"/>
       <c r="C109" s="4" t="s">
         <v>282</v>
       </c>
@@ -4036,7 +4042,7 @@
       <c r="E109" s="142"/>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B110" s="145"/>
+      <c r="B110" s="148"/>
       <c r="C110" s="4" t="s">
         <v>44</v>
       </c>
@@ -4046,7 +4052,7 @@
       <c r="E110" s="27"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B111" s="145"/>
+      <c r="B111" s="148"/>
       <c r="C111" s="4" t="s">
         <v>284</v>
       </c>
@@ -4056,7 +4062,7 @@
       <c r="E111" s="143"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B112" s="145"/>
+      <c r="B112" s="148"/>
       <c r="C112" s="4" t="s">
         <v>207</v>
       </c>
@@ -4066,7 +4072,7 @@
       <c r="E112" s="105"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B113" s="145"/>
+      <c r="B113" s="148"/>
       <c r="C113" s="4" t="s">
         <v>124</v>
       </c>
@@ -4076,7 +4082,7 @@
       <c r="E113" s="66"/>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B114" s="145"/>
+      <c r="B114" s="148"/>
       <c r="C114" s="4" t="s">
         <v>249</v>
       </c>
@@ -4086,7 +4092,7 @@
       <c r="E114" s="126"/>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B115" s="145"/>
+      <c r="B115" s="148"/>
       <c r="C115" s="4" t="s">
         <v>38</v>
       </c>
@@ -4096,7 +4102,7 @@
       <c r="E115" s="24"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B116" s="145"/>
+      <c r="B116" s="148"/>
       <c r="C116" s="4" t="s">
         <v>183</v>
       </c>
@@ -4106,7 +4112,7 @@
       <c r="E116" s="94"/>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B117" s="145"/>
+      <c r="B117" s="148"/>
       <c r="C117" s="4" t="s">
         <v>159</v>
       </c>
@@ -4116,7 +4122,7 @@
       <c r="E117" s="83"/>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B118" s="145"/>
+      <c r="B118" s="148"/>
       <c r="C118" s="4" t="s">
         <v>215</v>
       </c>
@@ -4126,7 +4132,7 @@
       <c r="E118" s="109"/>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B119" s="145"/>
+      <c r="B119" s="148"/>
       <c r="C119" s="4" t="s">
         <v>12</v>
       </c>
@@ -4136,7 +4142,7 @@
       <c r="E119" s="11"/>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B120" s="145"/>
+      <c r="B120" s="148"/>
       <c r="C120" s="4" t="s">
         <v>16</v>
       </c>
@@ -4146,17 +4152,17 @@
       <c r="E120" s="13"/>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B121" s="145"/>
+      <c r="B121" s="148"/>
       <c r="C121" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D121" s="146" t="s">
+      <c r="D121" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="E121" s="148"/>
+      <c r="E121" s="147"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B122" s="145"/>
+      <c r="B122" s="148"/>
       <c r="C122" s="4" t="s">
         <v>107</v>
       </c>
@@ -4166,7 +4172,7 @@
       <c r="E122" s="58"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B123" s="145"/>
+      <c r="B123" s="148"/>
       <c r="C123" s="4" t="s">
         <v>219</v>
       </c>
@@ -4176,7 +4182,7 @@
       <c r="E123" s="111"/>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B124" s="145"/>
+      <c r="B124" s="148"/>
       <c r="C124" s="4" t="s">
         <v>276</v>
       </c>
@@ -4186,7 +4192,7 @@
       <c r="E124" s="139"/>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B125" s="145"/>
+      <c r="B125" s="148"/>
       <c r="C125" s="4" t="s">
         <v>135</v>
       </c>
@@ -4196,7 +4202,7 @@
       <c r="E125" s="71"/>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B126" s="145"/>
+      <c r="B126" s="148"/>
       <c r="C126" s="4" t="s">
         <v>62</v>
       </c>
@@ -4206,7 +4212,7 @@
       <c r="E126" s="36"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B127" s="145"/>
+      <c r="B127" s="148"/>
       <c r="C127" s="4" t="s">
         <v>88</v>
       </c>
@@ -4216,7 +4222,7 @@
       <c r="E127" s="49"/>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B128" s="145"/>
+      <c r="B128" s="148"/>
       <c r="C128" s="4" t="s">
         <v>168</v>
       </c>
@@ -4226,7 +4232,7 @@
       <c r="E128" s="87"/>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B129" s="145"/>
+      <c r="B129" s="148"/>
       <c r="C129" s="4" t="s">
         <v>34</v>
       </c>
@@ -4236,7 +4242,7 @@
       <c r="E129" s="22"/>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B130" s="145"/>
+      <c r="B130" s="148"/>
       <c r="C130" s="4" t="s">
         <v>166</v>
       </c>
@@ -4246,7 +4252,7 @@
       <c r="E130" s="86"/>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B131" s="145"/>
+      <c r="B131" s="148"/>
       <c r="C131" s="4" t="s">
         <v>237</v>
       </c>
@@ -4256,7 +4262,7 @@
       <c r="E131" s="120"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B132" s="145"/>
+      <c r="B132" s="148"/>
       <c r="C132" s="4" t="s">
         <v>126</v>
       </c>
@@ -4266,7 +4272,7 @@
       <c r="E132" s="67"/>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B133" s="145"/>
+      <c r="B133" s="148"/>
       <c r="C133" s="4" t="s">
         <v>233</v>
       </c>
@@ -4276,7 +4282,7 @@
       <c r="E133" s="118"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B134" s="145"/>
+      <c r="B134" s="148"/>
       <c r="C134" s="4" t="s">
         <v>213</v>
       </c>
@@ -4286,7 +4292,7 @@
       <c r="E134" s="108"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B135" s="145"/>
+      <c r="B135" s="148"/>
       <c r="C135" s="4" t="s">
         <v>211</v>
       </c>
@@ -4296,7 +4302,7 @@
       <c r="E135" s="107"/>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B136" s="145"/>
+      <c r="B136" s="148"/>
       <c r="C136" s="4" t="s">
         <v>46</v>
       </c>
@@ -4306,7 +4312,7 @@
       <c r="E136" s="28"/>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B137" s="145"/>
+      <c r="B137" s="148"/>
       <c r="C137" s="4" t="s">
         <v>209</v>
       </c>
@@ -4316,7 +4322,7 @@
       <c r="E137" s="106"/>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B138" s="145"/>
+      <c r="B138" s="148"/>
       <c r="C138" s="4" t="s">
         <v>48</v>
       </c>
@@ -4326,7 +4332,7 @@
       <c r="E138" s="29"/>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B139" s="145"/>
+      <c r="B139" s="148"/>
       <c r="C139" s="4" t="s">
         <v>231</v>
       </c>
@@ -4336,7 +4342,7 @@
       <c r="E139" s="117"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B140" s="145"/>
+      <c r="B140" s="148"/>
       <c r="C140" s="4" t="s">
         <v>147</v>
       </c>
@@ -4346,7 +4352,7 @@
       <c r="E140" s="77"/>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B141" s="145"/>
+      <c r="B141" s="148"/>
       <c r="C141" s="4" t="s">
         <v>255</v>
       </c>
@@ -4356,7 +4362,7 @@
       <c r="E141" s="129"/>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B142" s="145"/>
+      <c r="B142" s="148"/>
       <c r="C142" s="4" t="s">
         <v>66</v>
       </c>
@@ -4366,7 +4372,7 @@
       <c r="E142" s="38"/>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B143" s="145"/>
+      <c r="B143" s="148"/>
       <c r="C143" s="4" t="s">
         <v>151</v>
       </c>
@@ -4376,7 +4382,7 @@
       <c r="E143" s="79"/>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B144" s="145"/>
+      <c r="B144" s="148"/>
       <c r="C144" s="4" t="s">
         <v>118</v>
       </c>
@@ -4386,7 +4392,7 @@
       <c r="E144" s="63"/>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B145" s="145"/>
+      <c r="B145" s="148"/>
       <c r="C145" s="4" t="s">
         <v>266</v>
       </c>
@@ -4396,7 +4402,7 @@
       <c r="E145" s="134"/>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B146" s="145"/>
+      <c r="B146" s="148"/>
       <c r="C146" s="4" t="s">
         <v>24</v>
       </c>
@@ -4406,7 +4412,7 @@
       <c r="E146" s="17"/>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B147" s="145"/>
+      <c r="B147" s="148"/>
       <c r="C147" s="4" t="s">
         <v>179</v>
       </c>
@@ -4416,7 +4422,7 @@
       <c r="E147" s="92"/>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B148" s="145"/>
+      <c r="B148" s="148"/>
       <c r="C148" s="4" t="s">
         <v>141</v>
       </c>
@@ -4426,7 +4432,7 @@
       <c r="E148" s="74"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B149" s="145"/>
+      <c r="B149" s="148"/>
       <c r="C149" s="4" t="s">
         <v>8</v>
       </c>
@@ -4436,12 +4442,12 @@
       <c r="E149" s="9"/>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B150" s="145"/>
+      <c r="B150" s="148"/>
       <c r="C150" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="D150" s="146"/>
-      <c r="E150" s="148"/>
+      <c r="D150" s="145"/>
+      <c r="E150" s="147"/>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B151" s="3"/>

</xml_diff>